<commit_message>
+ Added annotations for all the questions
</commit_message>
<xml_diff>
--- a/Data/output/Question2.xlsx
+++ b/Data/output/Question2.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <x:workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\UiPath\Shireen_Day_5\Data\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E14A03-B689-4D8B-B0AE-6CC2E9E0B0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView firstSheet="0" activeTab="0"/>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Landing" sheetId="2" r:id="rId2"/>
-    <x:sheet name="reading" sheetId="5" r:id="rId5"/>
-    <x:sheet name="inspirational" sheetId="7" r:id="rId7"/>
-    <x:sheet name="friendship" sheetId="8" r:id="rId8"/>
+    <x:sheet name="Landing" sheetId="2" r:id="rId1"/>
+    <x:sheet name="reading" sheetId="5" r:id="rId2"/>
+    <x:sheet name="inspirational" sheetId="7" r:id="rId3"/>
+    <x:sheet name="friendship" sheetId="8" r:id="rId4"/>
   </x:sheets>
   <x:definedNames/>
-  <x:calcPr calcId="125725"/>
+  <x:calcPr calcId="0"/>
 </x:workbook>
 </file>
 
@@ -256,13 +263,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="1" x14ac:knownFonts="1">
     <x:font>
-      <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
       <x:color rgb="FF000000"/>
       <x:name val="Calibri"/>
@@ -278,38 +284,32 @@
     </x:fill>
   </x:fills>
   <x:borders count="1">
-    <x:border diagonalUp="0" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="none">
-        <x:color rgb="FF000000"/>
-      </x:diagonal>
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
     </x:border>
   </x:borders>
   <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </x:cellStyleXfs>
   <x:cellXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </x:ext>
+  </x:extLst>
 </x:styleSheet>
 </file>
 
@@ -597,17 +597,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C10"/>
+  <x:dimension ref="A1"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="E17" sqref="E17 1:1048576"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -618,7 +620,7 @@
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:3">
+    <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
@@ -629,7 +631,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:3">
+    <x:row r="3" spans="1:5">
       <x:c r="A3" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -640,7 +642,7 @@
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:3">
+    <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
@@ -651,7 +653,7 @@
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:3">
+    <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -662,7 +664,7 @@
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:3">
+    <x:row r="6" spans="1:5">
       <x:c r="A6" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
@@ -673,7 +675,7 @@
         <x:v>16</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:3">
+    <x:row r="7" spans="1:5">
       <x:c r="A7" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
@@ -684,7 +686,7 @@
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:3">
+    <x:row r="8" spans="1:5">
       <x:c r="A8" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
@@ -695,7 +697,7 @@
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:3">
+    <x:row r="9" spans="1:5">
       <x:c r="A9" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
@@ -706,7 +708,7 @@
         <x:v>24</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:3">
+    <x:row r="10" spans="1:5">
       <x:c r="A10" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
@@ -717,7 +719,7 @@
         <x:v>27</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:3">
+    <x:row r="11" spans="1:5">
       <x:c r="A11" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -738,15 +740,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0100-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C7"/>
+  <x:dimension ref="A1"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="A1" sqref="A1 A1:C11"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:sheetData>
     <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">
@@ -846,15 +850,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0200-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C10"/>
+  <x:dimension ref="A1"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="A1" sqref="A1 A1:C11"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:sheetData>
     <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">
@@ -987,15 +993,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0300-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C5"/>
+  <x:dimension ref="A1"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A2" sqref="A2 A1:C11"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <x:sheetData>
     <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
+Changes made in question3
</commit_message>
<xml_diff>
--- a/Data/output/Question2.xlsx
+++ b/Data/output/Question2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <x:si>
     <x:t>Quotes</x:t>
   </x:si>
@@ -119,31 +119,34 @@
     <x:t>humor,obvious,simile</x:t>
   </x:si>
   <x:si>
-    <x:t>“The more that you read, the more things you will know. The more that you learn, the more places you'll go.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dr. Seuss</x:t>
-  </x:si>
-  <x:si>
-    <x:t>learning,reading,seuss</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“We read to know we're not alone.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>William Nicholson</x:t>
-  </x:si>
-  <x:si>
-    <x:t>misattributed-to-c-s-lewis,reading</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“A reader lives a thousand lives before he dies, said Jojen. The man who never reads lives only one.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>George R.R. Martin</x:t>
-  </x:si>
-  <x:si>
-    <x:t>read,readers,reading,reading-books</x:t>
+    <x:t>“This life is what you make it. No matter what, you're going to mess up sometimes, it's a universal truth. But the good part is you get to decide how you're going to mess it up. Girls will be your friends - they'll act like it anyway. But just remember, some come, some go. The ones that stay with you through everything - they're your true best friends. Don't let go of them. Also remember, sisters make the best friends in the world. As for lovers, well, they'll come and go too. And baby, I hate to say it, most of them - actually pretty much all of them are going to break your heart, but you can't give up because if you give up, you'll never find your soulmate. You'll never find that half who makes you whole and that goes for everything. Just because you fail once, doesn't mean you're gonna fail at everything. Keep trying, hold on, and always, always, always believe in yourself, because if you don't, then who will, sweetie? So keep your head high, keep your chin up, and most importantly, keep smiling, because life's a beautiful thing and there's so much to smile about.”</x:t>
+  </x:si>
+  <x:si>
+    <x:t>friends,heartbreak,inspirational,life,love,sisters</x:t>
+  </x:si>
+  <x:si>
+    <x:t>“The opposite of love is not hate, it's indifference. The opposite of art is not ugliness, it's indifference. The opposite of faith is not heresy, it's indifference. And the opposite of life is not death, it's indifference.”</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Elie Wiesel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>activism,apathy,hate,indifference,inspirational,love,opposite,philosophy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>“To the well-organized mind, death is but the next great adventure.”</x:t>
+  </x:si>
+  <x:si>
+    <x:t>death,inspirational</x:t>
+  </x:si>
+  <x:si>
+    <x:t>“It is never too late to be what you might have been.”</x:t>
+  </x:si>
+  <x:si>
+    <x:t>George Eliot</x:t>
+  </x:si>
+  <x:si>
+    <x:t>inspirational</x:t>
   </x:si>
   <x:si>
     <x:t>“You can never get a cup of tea large enough or a book long enough to suit me.”</x:t>
@@ -155,85 +158,34 @@
     <x:t>books,inspirational,reading,tea</x:t>
   </x:si>
   <x:si>
-    <x:t>“What really knocks me out is a book that, when you're all done reading it, you wish the author that wrote it was a terrific friend of yours and you could call him up on the phone whenever you felt like it. That doesn't happen much, though.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>J.D. Salinger</x:t>
-  </x:si>
-  <x:si>
-    <x:t>authors,books,literature,reading,writing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“′Classic′ - a book which people praise and don't read.”</x:t>
+    <x:t>“Only in the darkness can you see the stars.”</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Martin Luther King Jr.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hope,inspirational</x:t>
+  </x:si>
+  <x:si>
+    <x:t>“When one door of happiness closes, another opens; but often we look so long at the closed door that we do not see the one which has been opened for us.”</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Helen Keller</x:t>
+  </x:si>
+  <x:si>
+    <x:t>“It is not a lack of love, but a lack of friendship that makes unhappy marriages.”</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Friedrich Nietzsche</x:t>
+  </x:si>
+  <x:si>
+    <x:t>friendship,lack-of-friendship,lack-of-love,love,marriage,unhappy-marriage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>“Good friends, good books, and a sleepy conscience: this is the ideal life.”</x:t>
   </x:si>
   <x:si>
     <x:t>Mark Twain</x:t>
-  </x:si>
-  <x:si>
-    <x:t>books,classic,reading</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“I declare after all there is no enjoyment like reading! How much sooner one tires of any thing than of a book! -- When I have a house of my own, I shall be miserable if I have not an excellent library.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>books,library,reading</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“This life is what you make it. No matter what, you're going to mess up sometimes, it's a universal truth. But the good part is you get to decide how you're going to mess it up. Girls will be your friends - they'll act like it anyway. But just remember, some come, some go. The ones that stay with you through everything - they're your true best friends. Don't let go of them. Also remember, sisters make the best friends in the world. As for lovers, well, they'll come and go too. And baby, I hate to say it, most of them - actually pretty much all of them are going to break your heart, but you can't give up because if you give up, you'll never find your soulmate. You'll never find that half who makes you whole and that goes for everything. Just because you fail once, doesn't mean you're gonna fail at everything. Keep trying, hold on, and always, always, always believe in yourself, because if you don't, then who will, sweetie? So keep your head high, keep your chin up, and most importantly, keep smiling, because life's a beautiful thing and there's so much to smile about.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>friends,heartbreak,inspirational,life,love,sisters</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“The opposite of love is not hate, it's indifference. The opposite of art is not ugliness, it's indifference. The opposite of faith is not heresy, it's indifference. And the opposite of life is not death, it's indifference.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Elie Wiesel</x:t>
-  </x:si>
-  <x:si>
-    <x:t>activism,apathy,hate,indifference,inspirational,love,opposite,philosophy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“To the well-organized mind, death is but the next great adventure.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>death,inspirational</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“It is never too late to be what you might have been.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>George Eliot</x:t>
-  </x:si>
-  <x:si>
-    <x:t>inspirational</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“Only in the darkness can you see the stars.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Martin Luther King Jr.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>hope,inspirational</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“When one door of happiness closes, another opens; but often we look so long at the closed door that we do not see the one which has been opened for us.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Helen Keller</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“It is not a lack of love, but a lack of friendship that makes unhappy marriages.”</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Friedrich Nietzsche</x:t>
-  </x:si>
-  <x:si>
-    <x:t>friendship,lack-of-friendship,lack-of-love,love,marriage,unhappy-marriage</x:t>
-  </x:si>
-  <x:si>
-    <x:t>“Good friends, good books, and a sleepy conscience: this is the ideal life.”</x:t>
   </x:si>
   <x:si>
     <x:t>books,contentment,friends,friendship,life</x:t>
@@ -765,79 +717,112 @@
     </x:row>
     <x:row r="2" spans="1:3">
       <x:c r="A2" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
       <x:c r="A7" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
       <x:c r="A8" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:3">
+      <x:c r="A9" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:3">
+      <x:c r="A10" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:3">
+      <x:c r="A11" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>30</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -908,79 +893,79 @@
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>35</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:3">
       <x:c r="A7" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>37</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:3">
       <x:c r="A8" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:3">
       <x:c r="A9" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:3">
       <x:c r="A10" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3">
       <x:c r="A11" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1018,57 +1003,57 @@
     </x:row>
     <x:row r="2" spans="1:3">
       <x:c r="A2" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>51</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3">
       <x:c r="A3" s="0" t="s">
-        <x:v>69</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>70</x:v>
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s">
-        <x:v>71</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>72</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>57</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s">
-        <x:v>74</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:3">
       <x:c r="A6" s="0" t="s">
-        <x:v>76</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>77</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>75</x:v>
+        <x:v>59</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>